<commit_message>
Changes made to scoresheet and df plus ml docs
</commit_message>
<xml_diff>
--- a/Frontend/scorepredictions.xlsx
+++ b/Frontend/scorepredictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b631a87b7c0e187/Documents/VSCode/score_prediction_tool/Frontend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="11_68B48E941C65D00F6235547658A4163FBB38DE75" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B7DBD8A-1A57-4DD1-BC3F-10FE2140AD0F}"/>
+  <xr:revisionPtr revIDLastSave="479" documentId="11_68B48E941C65D00F6235547658A4163FBB38DE75" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA9DF759-362E-40DB-BA49-7CE5FA87A697}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="gamesheet_03-08-2024" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Team</t>
   </si>
@@ -208,6 +207,12 @@
   </si>
   <si>
     <t>AG?</t>
+  </si>
+  <si>
+    <t>BTTS?</t>
+  </si>
+  <si>
+    <t>BTTS p?</t>
   </si>
 </sst>
 </file>
@@ -228,7 +233,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +243,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,15 +289,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -607,7 +622,7 @@
     <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,8 +653,14 @@
       <c r="K1" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -673,8 +694,14 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -708,8 +735,14 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -743,8 +776,14 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -778,8 +817,14 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -813,8 +858,14 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -848,8 +899,14 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -883,8 +940,14 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -918,8 +981,14 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -953,8 +1022,14 @@
       <c r="K10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -988,8 +1063,14 @@
       <c r="K11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1023,8 +1104,14 @@
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1058,8 +1145,14 @@
       <c r="K13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1093,8 +1186,14 @@
       <c r="K14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1128,8 +1227,14 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1163,8 +1268,14 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1198,8 +1309,14 @@
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1233,8 +1350,14 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1268,8 +1391,14 @@
       <c r="K19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1303,8 +1432,14 @@
       <c r="K20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1338,8 +1473,14 @@
       <c r="K21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1373,8 +1514,14 @@
       <c r="K22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1408,8 +1555,14 @@
       <c r="K23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1443,8 +1596,14 @@
       <c r="K24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1478,8 +1637,14 @@
       <c r="K25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1513,8 +1678,14 @@
       <c r="K26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1548,8 +1719,14 @@
       <c r="K27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1583,8 +1760,14 @@
       <c r="K28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1618,8 +1801,14 @@
       <c r="K29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1653,8 +1842,14 @@
       <c r="K30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1688,8 +1883,14 @@
       <c r="K31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1723,8 +1924,14 @@
       <c r="K32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1758,8 +1965,14 @@
       <c r="K33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1793,8 +2006,14 @@
       <c r="K34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1828,8 +2047,14 @@
       <c r="K35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1863,8 +2088,14 @@
       <c r="K36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1898,8 +2129,14 @@
       <c r="K37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1933,8 +2170,14 @@
       <c r="K38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1968,8 +2211,14 @@
       <c r="K39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2003,8 +2252,14 @@
       <c r="K40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2038,8 +2293,14 @@
       <c r="K41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2073,8 +2334,14 @@
       <c r="K42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2108,8 +2375,14 @@
       <c r="K43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2143,8 +2416,14 @@
       <c r="K44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2178,8 +2457,14 @@
       <c r="K45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2213,8 +2498,14 @@
       <c r="K46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2248,8 +2539,14 @@
       <c r="K47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2283,8 +2580,14 @@
       <c r="K48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2318,8 +2621,14 @@
       <c r="K49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C50">
         <f t="shared" ref="C50:F50" si="0">SUM(C2:C49)</f>
         <v>73</v>
@@ -2353,11 +2662,19 @@
         <v>12</v>
       </c>
       <c r="K50">
-        <f t="shared" ref="K50" si="4">SUM(K2:K49)</f>
+        <f t="shared" ref="K50:M50" si="4">SUM(K2:K49)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L50" s="5">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C51">
         <f>C50/48</f>
         <v>1.5208333333333333</v>
@@ -2371,7 +2688,7 @@
         <v>12.5</v>
       </c>
       <c r="F51">
-        <f t="shared" ref="E51:K51" si="5">F50/48</f>
+        <f t="shared" ref="F51:G51" si="5">F50/48</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="G51">
@@ -2383,7 +2700,7 @@
         <v>47.916666666666671</v>
       </c>
       <c r="I51">
-        <f t="shared" ref="I51:K51" si="6">100*(I50/48)</f>
+        <f t="shared" ref="I51:M51" si="6">100*(I50/48)</f>
         <v>35.416666666666671</v>
       </c>
       <c r="J51">
@@ -2393,6 +2710,14 @@
       <c r="K51">
         <f t="shared" si="6"/>
         <v>35.416666666666671</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="6"/>
+        <v>79.166666666666657</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="6"/>
+        <v>47.916666666666671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes to dataframe and scoresheet code to work with run main
</commit_message>
<xml_diff>
--- a/Frontend/scorepredictions.xlsx
+++ b/Frontend/scorepredictions.xlsx
@@ -9,6 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gamesheet_03-08-2024" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gamesheet_03-14-2024" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gamesheet_03-28-2024" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gamesheet_04-03-2024" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -4271,4 +4272,1380 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Home Score</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Away Score</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>BTTS</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>First Goal Home</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>First Goal Away</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>Nation</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Arsenal v Luton</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Brentford v Brighton</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Manchester City v Aston Villa</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Liverpool v Sheffield United</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Chelsea v Manchester United</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Crystal Palace v Manchester City</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Aston Villa v Brentford</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Everton v Burnley</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Fulham v Newcastle United</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Luton v Bournemouth</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Wolverhampton Wanderers v West Ham</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Brighton v Arsenal</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Manchester United v Liverpool</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sheffield United v Chelsea</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Tottenham v Nottingham Forest</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>England</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Lille v Marseille</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Lens v Le Havre</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Paris Saint Germain v Clermont Foot</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Brest v Metz</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Montpellier v Lorient</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Reims v Nice</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Toulouse v Strasbourg</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Monaco v Rennes</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Nantes v Lyon</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Eintracht Frankfurt v Werder Bremen</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>FC Cologne v Bochum</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Freiburg v RasenBallsport Leipzig</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Mainz 05 v Darmstadt</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>3</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>FC Heidenheim v Bayern Munich</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Union Berlin v Bayer Leverkusen</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Borussia Dortmund v VfB Stuttgart</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Hoffenheim v Augsburg</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Wolfsburg v Borussia M.Gladbach</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Salernitana v Sassuolo</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>AC Milan v Lecce</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Roma v Lazio</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>2</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Empoli v Torino</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Frosinone v Bologna</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Monza v Napoli</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Cagliari v Atalanta</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Verona v Genoa</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Juventus v Fiorentina</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>2</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Udinese v Inter</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Granada v Valencia</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>